<commit_message>
admin exclue list date &time functionality
 admin exclue list date &time functionality
</commit_message>
<xml_diff>
--- a/assets/modality_list.xlsx
+++ b/assets/modality_list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Test Type</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>FEVER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blood </t>
   </si>
 </sst>
 </file>
@@ -511,7 +508,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>

</xml_diff>